<commit_message>
[FEATURE] Bloqueo y Desbloqueo
Se agregaron dos casos al modulo y se ajusto configuracion a la base de
datos
</commit_message>
<xml_diff>
--- a/Test Data/Datos conexion BD.xlsx
+++ b/Test Data/Datos conexion BD.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20402"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Franco.Mallea\AppData\Roaming\Microsoft\Windows\Network Shortcuts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guillermo.Ameztoy\git\Crecer\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A5DB5BE-F79E-4C41-BAC2-5026BD7679C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3074A419-8E39-42CB-8BA4-C1C96EC60740}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{B974CCA0-A1AD-4538-957F-D41159EB01D1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Database" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,13 +48,13 @@
     <t>dBUser</t>
   </si>
   <si>
-    <t>gnoh3ul6ltj5e8xsaz0i</t>
-  </si>
-  <si>
     <t>dBPass</t>
   </si>
   <si>
-    <t>pscale_pw_SC9qrsEQ81zydy07vCqPnX1crVStaiS4JN1Oxsf9d5q</t>
+    <t>po3v5snd2tli5v86ntwo</t>
+  </si>
+  <si>
+    <t>pscale_pw_WDxyGqANy4q29eTUirqYuwo29kwRzaEJFWuO6f0uKqP</t>
   </si>
 </sst>
 </file>
@@ -408,9 +408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1B8C308-8018-414D-B4F4-F7F7144AA1B8}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -447,12 +445,12 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
[UPDATE] Datos de conexion a la base de datos
</commit_message>
<xml_diff>
--- a/Test Data/Datos conexion BD.xlsx
+++ b/Test Data/Datos conexion BD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guillermo.Ameztoy\git\Crecer\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3074A419-8E39-42CB-8BA4-C1C96EC60740}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F814DBB3-F0D6-4776-827D-53405A44E408}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{B974CCA0-A1AD-4538-957F-D41159EB01D1}"/>
   </bookViews>
@@ -51,10 +51,10 @@
     <t>dBPass</t>
   </si>
   <si>
-    <t>po3v5snd2tli5v86ntwo</t>
-  </si>
-  <si>
-    <t>pscale_pw_WDxyGqANy4q29eTUirqYuwo29kwRzaEJFWuO6f0uKqP</t>
+    <t>eychrqfbwkj65rqogd77</t>
+  </si>
+  <si>
+    <t>pscale_pw_XMsJE9uSyMrK7NnecpXf71tNHNhUrMmf9sdRdIOuPim</t>
   </si>
 </sst>
 </file>
@@ -408,7 +408,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1B8C308-8018-414D-B4F4-F7F7144AA1B8}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
[UPDATE] Datos conexion BD + Renombre objetos Alta de Cuentas
</commit_message>
<xml_diff>
--- a/Test Data/Datos conexion BD.xlsx
+++ b/Test Data/Datos conexion BD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guillermo.Ameztoy\git\Crecer\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F814DBB3-F0D6-4776-827D-53405A44E408}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{778A8A61-EB8E-4613-9F85-67185550F893}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{B974CCA0-A1AD-4538-957F-D41159EB01D1}"/>
   </bookViews>
@@ -51,10 +51,10 @@
     <t>dBPass</t>
   </si>
   <si>
-    <t>eychrqfbwkj65rqogd77</t>
-  </si>
-  <si>
-    <t>pscale_pw_XMsJE9uSyMrK7NnecpXf71tNHNhUrMmf9sdRdIOuPim</t>
+    <t>pscale_pw_8lmwdeLbOlpwgLrIVyJNwhmmNZfq3xTokRdG8IuZ34O</t>
+  </si>
+  <si>
+    <t>kqg4sm1ik53xfqvs984d</t>
   </si>
 </sst>
 </file>
@@ -409,7 +409,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,7 +447,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -455,7 +455,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[UPDATE] DB user and pass
</commit_message>
<xml_diff>
--- a/Test Data/Datos conexion BD.xlsx
+++ b/Test Data/Datos conexion BD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guillermo.Ameztoy\git\Crecer\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{778A8A61-EB8E-4613-9F85-67185550F893}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC061AB4-0FBD-4B33-82C7-17275731A444}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{B974CCA0-A1AD-4538-957F-D41159EB01D1}"/>
   </bookViews>
@@ -51,10 +51,10 @@
     <t>dBPass</t>
   </si>
   <si>
-    <t>pscale_pw_8lmwdeLbOlpwgLrIVyJNwhmmNZfq3xTokRdG8IuZ34O</t>
-  </si>
-  <si>
-    <t>kqg4sm1ik53xfqvs984d</t>
+    <t>pscale_pw_sQC7AtS7wbLZ9gGW5DVfRwcWG0dwjuNMkoZdteZd2qL</t>
+  </si>
+  <si>
+    <t>e8uheosght0rud322qr2</t>
   </si>
 </sst>
 </file>
@@ -409,7 +409,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>